<commit_message>
PyTessaract changes and code stabilization
</commit_message>
<xml_diff>
--- a/devdata/input/OWN FLEET TESTING CUSTOMER LIST 2024-07.xlsx
+++ b/devdata/input/OWN FLEET TESTING CUSTOMER LIST 2024-07.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\27810\source\repos\robots\techfinity-orders-robot\devdata\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D054886-8F6F-429B-BA39-FBCA9F10CA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C41C5F7-7DEE-4D74-BE9B-66735D4E3551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F2BA53A3-BB35-4397-B792-2E6C42BA57DE}"/>
   </bookViews>
@@ -155,9 +155,6 @@
     <t>5.34</t>
   </si>
   <si>
-    <t>BRMD</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -171,6 +168,9 @@
   </si>
   <si>
     <t>TEST</t>
+  </si>
+  <si>
+    <t>BRM</t>
   </si>
 </sst>
 </file>
@@ -617,7 +617,7 @@
   <dimension ref="A1:AD1558"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -670,10 +670,10 @@
         <v>35</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>36</v>
@@ -744,10 +744,10 @@
         <v>21</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C2" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>37</v>
@@ -759,13 +759,13 @@
         <v>38</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J2" s="5">
         <v>1992</v>

</xml_diff>

<commit_message>
Get PNUMBER and Test each module
</commit_message>
<xml_diff>
--- a/devdata/input/OWN FLEET TESTING CUSTOMER LIST 2024-07.xlsx
+++ b/devdata/input/OWN FLEET TESTING CUSTOMER LIST 2024-07.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\27810\source\repos\robots\techfinity-orders-robot\devdata\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C41C5F7-7DEE-4D74-BE9B-66735D4E3551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041E2995-742F-42DE-8431-5C3A85DB8E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F2BA53A3-BB35-4397-B792-2E6C42BA57DE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t>Account No</t>
   </si>
@@ -147,9 +147,6 @@
   </si>
   <si>
     <t>Checker</t>
-  </si>
-  <si>
-    <t>C22</t>
   </si>
   <si>
     <t>5.34</t>
@@ -617,13 +614,15 @@
   <dimension ref="A1:AD1558"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="10.44140625" customWidth="1"/>
+    <col min="2" max="3" width="10.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="11" customWidth="1"/>
     <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
@@ -670,10 +669,10 @@
         <v>35</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>36</v>
@@ -744,28 +743,28 @@
         <v>21</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="5">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>37</v>
+      <c r="D2" s="5">
+        <v>22</v>
       </c>
       <c r="E2" s="5">
         <v>1</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J2" s="5">
         <v>1992</v>

</xml_diff>